<commit_message>
Auto-committed on 2021/12/10 週五
Former-commit-id: c106389a49a84c13c5a91b6c8602f0f892129457
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/JobDetail.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/JobDetail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L6-共同作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C135EF-9428-4AC4-8007-4BA32BE3DAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10497522-23C1-4F4C-BB21-843AC845581C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="108" windowWidth="17568" windowHeight="11532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -310,6 +310,26 @@
   </si>
   <si>
     <t>ExecDate DESC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>findExecDateIn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ExecDate &gt;= ,AND ExecDate &lt;= </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StepStartTime DESC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>findStatusExecDateIn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExecDate &gt;= ,AND ExecDate &lt;= ,AND Status =</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -940,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1344,16 +1364,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="67.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
@@ -1401,6 +1421,28 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2021/12/24 週五
Former-commit-id: 613868152d69622e600a590d83c3b2865962293d
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/JobDetail.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/JobDetail.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L6-共同作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10497522-23C1-4F4C-BB21-843AC845581C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -336,12 +335,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -349,7 +348,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -383,7 +382,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -412,7 +411,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -507,7 +506,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -618,11 +617,14 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -713,23 +715,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -765,23 +750,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -957,25 +925,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.25" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.25" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.77734375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="21.44140625" style="7"/>
+    <col min="7" max="7" width="42.75" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="21.5" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="33" t="s">
         <v>8</v>
       </c>
@@ -990,7 +958,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="33"/>
       <c r="B2" s="34"/>
       <c r="C2" s="8" t="s">
@@ -1003,7 +971,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
@@ -1018,7 +986,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="33" t="s">
         <v>11</v>
       </c>
@@ -1033,7 +1001,7 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="36" t="s">
         <v>5</v>
       </c>
@@ -1044,7 +1012,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="33" t="s">
         <v>6</v>
       </c>
@@ -1055,7 +1023,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1034,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="15" customFormat="1">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1057,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="20" customFormat="1">
       <c r="A9" s="16">
         <v>1</v>
       </c>
@@ -1110,7 +1078,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="16">
         <v>2</v>
       </c>
@@ -1131,7 +1099,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="20" customFormat="1">
       <c r="A11" s="16">
         <v>3</v>
       </c>
@@ -1152,7 +1120,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="33">
       <c r="A12" s="16">
         <v>4</v>
       </c>
@@ -1173,7 +1141,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="33">
       <c r="A13" s="16">
         <v>5</v>
       </c>
@@ -1194,7 +1162,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="49.5">
       <c r="A14" s="16">
         <v>6</v>
       </c>
@@ -1215,7 +1183,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" s="16">
         <v>7</v>
       </c>
@@ -1236,7 +1204,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="16">
         <v>8</v>
       </c>
@@ -1249,13 +1217,12 @@
       <c r="D16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="29"/>
       <c r="F16" s="30"/>
       <c r="G16" s="21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" s="16">
         <v>9</v>
       </c>
@@ -1268,13 +1235,12 @@
       <c r="D17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="29"/>
       <c r="F17" s="30"/>
       <c r="G17" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="16">
         <v>10</v>
       </c>
@@ -1287,13 +1253,13 @@
       <c r="D18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="37">
         <v>6</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="16">
         <v>11</v>
       </c>
@@ -1306,11 +1272,11 @@
       <c r="D19" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="31"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="31"/>
       <c r="G19" s="22"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" s="16">
         <v>12</v>
       </c>
@@ -1323,13 +1289,13 @@
       <c r="D20" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="37">
         <v>6</v>
       </c>
       <c r="F20" s="31"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="26" customFormat="1">
       <c r="A21" s="16">
         <v>13</v>
       </c>
@@ -1342,7 +1308,7 @@
       <c r="D21" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="31"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="31"/>
       <c r="G21" s="25"/>
     </row>
@@ -1363,23 +1329,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="25.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="67.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.75" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1390,7 +1356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -1401,7 +1367,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -1412,7 +1378,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -1423,7 +1389,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>73</v>
       </c>
@@ -1434,7 +1400,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
@@ -1453,23 +1419,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="6" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.875" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="6" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="27" customFormat="1">
       <c r="A1" s="27" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Auto-committed on 2021/12/29 週三
Former-commit-id: ee1eeebf4bba752005065e5c4402d09963217b10
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/JobDetail.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/JobDetail.xlsx
@@ -168,10 +168,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>JobDetail</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>批次工作明細檔</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -336,6 +332,9 @@
   </si>
   <si>
     <t>TxSeq,ExecDate,JobCode</t>
+  </si>
+  <si>
+    <t>JobDetail</t>
   </si>
 </sst>
 </file>
@@ -615,6 +614,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -626,9 +628,6 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -938,7 +937,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="16.5"/>
@@ -953,23 +952,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
@@ -981,12 +980,12 @@
       <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>13</v>
@@ -995,26 +994,26 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" ht="33">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="37"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="10"/>
@@ -1022,10 +1021,10 @@
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="3"/>
       <c r="D6" s="13"/>
       <c r="E6" s="10"/>
@@ -1033,10 +1032,10 @@
       <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="3"/>
       <c r="D7" s="13"/>
       <c r="E7" s="10"/>
@@ -1067,23 +1066,23 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="20" customFormat="1">
-      <c r="A9" s="38">
+      <c r="A9" s="34">
         <v>1</v>
       </c>
       <c r="B9" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="38">
+      <c r="E9" s="34">
         <v>20</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="20" customFormat="1">
@@ -1091,10 +1090,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>32</v>
@@ -1104,7 +1103,7 @@
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1133,10 +1132,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>12</v>
@@ -1146,7 +1145,7 @@
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="33">
@@ -1154,20 +1153,20 @@
         <v>4</v>
       </c>
       <c r="B13" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="E13" s="32">
         <v>1</v>
       </c>
       <c r="F13" s="30"/>
       <c r="G13" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="33">
@@ -1175,20 +1174,20 @@
         <v>5</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="16">
         <v>1</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="49.5">
@@ -1196,20 +1195,20 @@
         <v>6</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>50</v>
-      </c>
       <c r="D15" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="16">
         <v>15</v>
       </c>
       <c r="F15" s="30"/>
       <c r="G15" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1217,20 +1216,20 @@
         <v>7</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>53</v>
-      </c>
       <c r="D16" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="16">
         <v>3000</v>
       </c>
       <c r="F16" s="30"/>
       <c r="G16" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1238,17 +1237,17 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1256,17 +1255,17 @@
         <v>9</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1387,57 +1386,57 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>